<commit_message>
Finale Version 2.0.0 Projektantrag
Projektantrag finalisiert.
Zeitaufzeichnung aktualisiert
</commit_message>
<xml_diff>
--- a/Zeitaufzeichnung.xlsx
+++ b/Zeitaufzeichnung.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\workspace\school\SEW\gitrep\School-Quakes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Desktop\4CHIT\ITP\Rafeiner-Magor\School-Quakes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -483,15 +483,15 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="11.42578125" style="1"/>
+    <col min="6" max="6" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,7 +499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -507,10 +507,10 @@
         <v>4.5</v>
       </c>
       <c r="H2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -521,7 +521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -532,7 +532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -540,10 +540,10 @@
         <v>7</v>
       </c>
       <c r="H5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -555,10 +555,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B7" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -569,18 +569,18 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H10" s="4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -591,7 +591,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>13</v>
       </c>
@@ -602,7 +602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>14</v>
       </c>
@@ -613,7 +613,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>15</v>
       </c>
@@ -624,94 +624,94 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Lastenheft 1.0.0 Finale Version
Fertigstellung des Lastenheftes
+Änderung der Zeiteinschätzung
</commit_message>
<xml_diff>
--- a/Zeitaufzeichnung.xlsx
+++ b/Zeitaufzeichnung.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Limbeck\Desktop\Schule 15-16\Projekt\Schools &amp; Quakes\School &amp; Quakes Projekt-Repository\School-Quakes\School-Quakes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\workspace\school\SEW\gitrep\School-Quakes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Durchgeführt</t>
   </si>
@@ -44,15 +44,9 @@
     <t>Projektkoordination</t>
   </si>
   <si>
-    <t>bis jetzt 1</t>
-  </si>
-  <si>
     <t>Projektcontroling</t>
   </si>
   <si>
-    <t>bis jetzt 2</t>
-  </si>
-  <si>
     <t>Projektabschluss</t>
   </si>
   <si>
@@ -128,7 +122,10 @@
     <t>Abnahme</t>
   </si>
   <si>
-    <t>bis jz 8,5</t>
+    <t>bis jetzt 3</t>
+  </si>
+  <si>
+    <t>bis jetzt 1,5</t>
   </si>
 </sst>
 </file>
@@ -483,15 +480,15 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="11.453125" style="1"/>
+    <col min="6" max="6" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,7 +496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -510,7 +507,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -521,31 +518,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="H4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="H5">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F6" s="1">
         <f>[1]Projektmanagement!J5</f>
@@ -555,23 +552,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F9" s="1">
-        <v>4</v>
+        <v>11.5</v>
       </c>
       <c r="H9" s="4">
         <v>21.5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F10" s="1">
         <v>2</v>
@@ -580,20 +577,20 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>33</v>
+        <v>9</v>
+      </c>
+      <c r="F11" s="1">
+        <v>9.5</v>
       </c>
       <c r="H11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -602,9 +599,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -613,9 +610,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
@@ -624,96 +621,96 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B17" s="2" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B21" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B23" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B25" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B26" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B28" s="2" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B29" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B30" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B31" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B33" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>